<commit_message>
Feat: updated set_up_mets to include measured column
This column specifies whether or not a metabolite was measured.
This is important to sample metabolite concentrations, giving
higher priority to measured metabolites vs. unmeasured ones.
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/model_v1_manual2_EX.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_set_up_models/set_up_model/model_v1_manual2_EX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="389">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>fixed?</t>
+  </si>
+  <si>
+    <t>measured?</t>
   </si>
   <si>
     <t>D-glucose extracellular</t>
@@ -1342,7 +1345,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="1" sqref="1:1 G30"/>
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1472,30 +1475,30 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="1" sqref="1:1 A38"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,7 +2498,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="1" sqref="1:1 A38"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2505,16 +2508,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3110,7 +3113,7 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3120,16 +3123,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3752,88 +3755,88 @@
   </sheetPr>
   <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3841,13 +3844,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -3859,10 +3862,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -3874,10 +3877,10 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
@@ -3888,13 +3891,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -3906,10 +3909,10 @@
         <v>1</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
@@ -3921,10 +3924,10 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
@@ -3935,13 +3938,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -3953,10 +3956,10 @@
         <v>2</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -3968,10 +3971,10 @@
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
@@ -3982,7 +3985,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
@@ -4009,10 +4012,10 @@
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
@@ -4023,13 +4026,13 @@
         <v>73</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -4044,13 +4047,13 @@
         <v>2</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="S6" s="4" t="n">
         <v>5470828</v>
@@ -4059,10 +4062,10 @@
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
@@ -4073,10 +4076,10 @@
         <v>74</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>29</v>
@@ -4091,10 +4094,10 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
@@ -4105,13 +4108,13 @@
         <v>75</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -4123,13 +4126,13 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Z8" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
@@ -4139,16 +4142,16 @@
         <v>76</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -4166,16 +4169,16 @@
         <v>77</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>281</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -4186,10 +4189,10 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
@@ -4199,13 +4202,13 @@
         <v>78</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -4213,23 +4216,23 @@
         <v>1</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="T11" s="4"/>
       <c r="V11" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="X11" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
@@ -4239,13 +4242,13 @@
         <v>79</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -4254,13 +4257,13 @@
       </c>
       <c r="T12" s="4"/>
       <c r="X12" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
@@ -4270,16 +4273,16 @@
         <v>80</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G13" s="4"/>
       <c r="I13" s="4" t="s">
@@ -4292,37 +4295,37 @@
         <v>2</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="U13" s="4" t="n">
         <v>6815421</v>
       </c>
       <c r="V13" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W13" s="4" t="n">
         <v>6815421</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
@@ -4332,19 +4335,19 @@
         <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
@@ -4360,31 +4363,31 @@
         <v>2</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="U14" s="4" t="n">
         <v>6815421</v>
       </c>
       <c r="V14" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W14" s="4" t="n">
         <v>6815421</v>
@@ -4397,19 +4400,19 @@
         <v>82</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4" t="s">
@@ -4425,48 +4428,48 @@
         <v>2</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="U15" s="4" t="n">
         <v>6815421</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W15" s="4" t="n">
         <v>6815421</v>
       </c>
       <c r="X15" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>37</v>
@@ -4479,10 +4482,10 @@
         <v>1</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4490,16 +4493,16 @@
         <v>84</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>33</v>
@@ -4509,25 +4512,25 @@
         <v>2</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M17" s="4" t="n">
         <v>19686854</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="O17" s="4" t="n">
         <v>4154932</v>
       </c>
       <c r="V17" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W17" s="4" t="n">
         <v>19686854</v>
       </c>
       <c r="X17" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4535,16 +4538,16 @@
         <v>85</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>33</v>
@@ -4554,25 +4557,25 @@
         <v>2</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M18" s="4" t="n">
         <v>19686854</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="O18" s="4" t="n">
         <v>4154932</v>
       </c>
       <c r="V18" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W18" s="4" t="n">
         <v>19686854</v>
       </c>
       <c r="X18" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4580,10 +4583,10 @@
         <v>86</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>40</v>
@@ -4593,13 +4596,13 @@
         <v>2</v>
       </c>
       <c r="V19" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="Y19" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4607,29 +4610,29 @@
         <v>87</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G20" s="4"/>
       <c r="K20" s="4" t="n">
         <v>2</v>
       </c>
       <c r="V20" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="X20" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y20" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4637,35 +4640,35 @@
         <v>88</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G21" s="4"/>
       <c r="K21" s="4" t="n">
         <v>2</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M21" s="4" t="n">
         <v>17914867</v>
       </c>
       <c r="V21" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="X21" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="Y21" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4673,35 +4676,35 @@
         <v>89</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G22" s="4"/>
       <c r="K22" s="4" t="n">
         <v>2</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M22" s="4" t="n">
         <v>17914867</v>
       </c>
       <c r="V22" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="X22" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="Y22" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4709,35 +4712,35 @@
         <v>90</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G23" s="4"/>
       <c r="K23" s="4" t="n">
         <v>2</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M23" s="4" t="n">
         <v>8805555</v>
       </c>
       <c r="V23" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="X23" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4745,7 +4748,7 @@
         <v>91</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>27</v>
@@ -4760,22 +4763,22 @@
         <v>2</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="O24" s="4" t="n">
         <v>4154932</v>
       </c>
       <c r="V24" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W24" s="4" t="n">
         <v>6326623</v>
       </c>
       <c r="X24" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y24" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4783,34 +4786,34 @@
         <v>92</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K25" s="4" t="n">
         <v>3</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W25" s="4" t="n">
         <v>12876349</v>
       </c>
       <c r="X25" s="4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4818,7 +4821,7 @@
         <v>93</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>24</v>
@@ -4830,16 +4833,16 @@
         <v>2</v>
       </c>
       <c r="V26" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="X26" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4847,28 +4850,28 @@
         <v>94</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K27" s="4" t="n">
         <v>4</v>
       </c>
       <c r="V27" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="X27" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Y27" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4876,10 +4879,10 @@
         <v>95</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>48</v>
@@ -4888,22 +4891,22 @@
         <v>4</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="V28" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="X28" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4911,7 +4914,7 @@
         <v>96</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>42</v>
@@ -4923,16 +4926,16 @@
         <v>2</v>
       </c>
       <c r="V29" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="X29" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="Y29" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4940,13 +4943,13 @@
         <v>97</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>54</v>
@@ -4958,22 +4961,22 @@
         <v>4</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M30" s="4" t="n">
         <v>7447472</v>
       </c>
       <c r="V30" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W30" s="4" t="n">
         <v>8636984</v>
       </c>
       <c r="X30" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4981,34 +4984,34 @@
         <v>98</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="K31" s="4" t="n">
         <v>1</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M31" s="4" t="n">
         <v>5128739</v>
       </c>
       <c r="V31" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="X31" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y31" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5016,7 +5019,7 @@
         <v>99</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>51</v>
@@ -5028,19 +5031,19 @@
         <v>1</v>
       </c>
       <c r="V32" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="W32" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="X32" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="Y32" s="4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z32" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5048,7 +5051,7 @@
         <v>100</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>52</v>
@@ -5060,16 +5063,16 @@
         <v>2</v>
       </c>
       <c r="V33" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W33" s="4" t="n">
         <v>9376357</v>
       </c>
       <c r="X33" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="Y33" s="4" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5077,16 +5080,16 @@
         <v>101</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="J34" s="4" t="n">
         <v>4</v>
@@ -5095,28 +5098,28 @@
         <v>4</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="T34" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="U34" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="V34" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="W34" s="4" t="n">
         <v>468836</v>
       </c>
       <c r="X34" s="4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5124,10 +5127,10 @@
         <v>102</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>56</v>
@@ -5136,16 +5139,16 @@
         <v>1</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="V35" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5153,28 +5156,28 @@
         <v>103</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="K36" s="4" t="n">
         <v>1</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="V36" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="W36" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5182,7 +5185,7 @@
         <v>104</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="K37" s="4" t="n">
         <v>1</v>
@@ -5193,7 +5196,7 @@
         <v>105</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="K38" s="4" t="n">
         <v>1</v>
@@ -5204,7 +5207,7 @@
         <v>106</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="K39" s="4" t="n">
         <v>1</v>
@@ -5215,7 +5218,7 @@
         <v>107</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>47</v>
@@ -5244,7 +5247,7 @@
       <c r="V40" s="4"/>
       <c r="W40" s="4"/>
       <c r="X40" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="Y40" s="4"/>
       <c r="Z40" s="4"/>
@@ -5256,7 +5259,7 @@
         <v>108</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>53</v>
@@ -5285,7 +5288,7 @@
       <c r="V41" s="4"/>
       <c r="W41" s="4"/>
       <c r="X41" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="Y41" s="4"/>
       <c r="Z41" s="4"/>
@@ -5297,7 +5300,7 @@
         <v>109</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>60</v>
@@ -5327,7 +5330,7 @@
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
       <c r="X42" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
@@ -5359,7 +5362,7 @@
   <dimension ref="1:50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="1" sqref="1:1 A38"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -61883,15 +61886,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="1" sqref="1:1 H11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -61911,13 +61914,16 @@
       <c r="E1" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>0</v>
@@ -61927,6 +61933,9 @@
       </c>
       <c r="E2" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -61934,7 +61943,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>1</v>
@@ -61943,6 +61952,9 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -61951,7 +61963,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>1</v>
@@ -61961,6 +61973,9 @@
       </c>
       <c r="E4" s="4" t="n">
         <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -61968,7 +61983,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>1</v>
@@ -61977,6 +61992,9 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -61985,7 +62003,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>1</v>
@@ -61995,6 +62013,9 @@
       </c>
       <c r="E6" s="4" t="n">
         <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62002,7 +62023,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>0</v>
@@ -62012,6 +62033,9 @@
       </c>
       <c r="E7" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62019,7 +62043,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>1</v>
@@ -62028,6 +62052,9 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62036,7 +62063,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>1</v>
@@ -62045,6 +62072,9 @@
         <v>1</v>
       </c>
       <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62053,7 +62083,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>1</v>
@@ -62063,6 +62093,9 @@
       </c>
       <c r="E10" s="4" t="n">
         <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62070,7 +62103,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>1</v>
@@ -62079,6 +62112,9 @@
         <v>1</v>
       </c>
       <c r="E11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62087,7 +62123,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>1</v>
@@ -62096,6 +62132,9 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62104,7 +62143,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>1</v>
@@ -62113,6 +62152,9 @@
         <v>1</v>
       </c>
       <c r="E13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62121,7 +62163,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>1</v>
@@ -62130,6 +62172,9 @@
         <v>1</v>
       </c>
       <c r="E14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62138,7 +62183,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>1</v>
@@ -62147,6 +62192,9 @@
         <v>1</v>
       </c>
       <c r="E15" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62155,7 +62203,7 @@
         <v>32</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>1</v>
@@ -62164,6 +62212,9 @@
         <v>1</v>
       </c>
       <c r="E16" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62172,7 +62223,7 @@
         <v>33</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>1</v>
@@ -62181,6 +62232,9 @@
         <v>1</v>
       </c>
       <c r="E17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62189,7 +62243,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>1</v>
@@ -62198,6 +62252,9 @@
         <v>1</v>
       </c>
       <c r="E18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62206,7 +62263,7 @@
         <v>35</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>0</v>
@@ -62215,6 +62272,9 @@
         <v>1</v>
       </c>
       <c r="E19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -62223,7 +62283,7 @@
         <v>36</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>0</v>
@@ -62233,6 +62293,9 @@
       </c>
       <c r="E20" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62240,7 +62303,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>1</v>
@@ -62249,6 +62312,9 @@
         <v>1</v>
       </c>
       <c r="E21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62257,7 +62323,7 @@
         <v>38</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>0</v>
@@ -62267,6 +62333,9 @@
       </c>
       <c r="E22" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62274,7 +62343,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>1</v>
@@ -62283,6 +62352,9 @@
         <v>1</v>
       </c>
       <c r="E23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62291,7 +62363,7 @@
         <v>40</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>1</v>
@@ -62300,6 +62372,9 @@
         <v>1</v>
       </c>
       <c r="E24" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62308,7 +62383,7 @@
         <v>41</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>1</v>
@@ -62317,6 +62392,9 @@
         <v>1</v>
       </c>
       <c r="E25" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62325,7 +62403,7 @@
         <v>42</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>1</v>
@@ -62335,6 +62413,9 @@
       </c>
       <c r="E26" s="4" t="n">
         <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62342,7 +62423,7 @@
         <v>43</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>1</v>
@@ -62351,6 +62432,9 @@
         <v>1</v>
       </c>
       <c r="E27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62359,7 +62443,7 @@
         <v>44</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>1</v>
@@ -62368,6 +62452,9 @@
         <v>1</v>
       </c>
       <c r="E28" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62376,7 +62463,7 @@
         <v>45</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>1</v>
@@ -62385,6 +62472,9 @@
         <v>1</v>
       </c>
       <c r="E29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62393,7 +62483,7 @@
         <v>46</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>1</v>
@@ -62402,6 +62492,9 @@
         <v>1</v>
       </c>
       <c r="E30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62410,7 +62503,7 @@
         <v>47</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>1</v>
@@ -62419,6 +62512,9 @@
         <v>1</v>
       </c>
       <c r="E31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62427,7 +62523,7 @@
         <v>48</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>1</v>
@@ -62436,6 +62532,9 @@
         <v>1</v>
       </c>
       <c r="E32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62444,7 +62543,7 @@
         <v>49</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>1</v>
@@ -62453,6 +62552,9 @@
         <v>1</v>
       </c>
       <c r="E33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62461,7 +62563,7 @@
         <v>50</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>1</v>
@@ -62470,6 +62572,9 @@
         <v>1</v>
       </c>
       <c r="E34" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62478,7 +62583,7 @@
         <v>51</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>1</v>
@@ -62487,6 +62592,9 @@
         <v>1</v>
       </c>
       <c r="E35" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62495,7 +62603,7 @@
         <v>52</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>1</v>
@@ -62505,6 +62613,9 @@
       </c>
       <c r="E36" s="4" t="n">
         <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62512,7 +62623,7 @@
         <v>53</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>1</v>
@@ -62521,6 +62632,9 @@
         <v>1</v>
       </c>
       <c r="E37" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62529,7 +62643,7 @@
         <v>54</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>1</v>
@@ -62538,6 +62652,9 @@
         <v>1</v>
       </c>
       <c r="E38" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62546,7 +62663,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>1</v>
@@ -62555,6 +62672,9 @@
         <v>1</v>
       </c>
       <c r="E39" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62563,7 +62683,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>1</v>
@@ -62572,6 +62692,9 @@
         <v>1</v>
       </c>
       <c r="E40" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -62580,7 +62703,7 @@
         <v>57</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>0</v>
@@ -62590,6 +62713,9 @@
       </c>
       <c r="E41" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62597,7 +62723,7 @@
         <v>58</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>0</v>
@@ -62607,6 +62733,9 @@
       </c>
       <c r="E42" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62614,7 +62743,7 @@
         <v>59</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>0</v>
@@ -62624,6 +62753,9 @@
       </c>
       <c r="E43" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62631,7 +62763,7 @@
         <v>60</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>0</v>
@@ -62641,6 +62773,9 @@
       </c>
       <c r="E44" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -62662,12 +62797,12 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="1" sqref="1:1 A38"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -62676,16 +62811,16 @@
         <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62693,7 +62828,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>0</v>
@@ -62707,7 +62842,7 @@
         <v>70</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>0</v>
@@ -62721,7 +62856,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>0</v>
@@ -62735,7 +62870,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>0</v>
@@ -62749,7 +62884,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>0</v>
@@ -62763,7 +62898,7 @@
         <v>74</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>0</v>
@@ -62777,7 +62912,7 @@
         <v>75</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>0</v>
@@ -62791,7 +62926,7 @@
         <v>76</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>0</v>
@@ -62805,7 +62940,7 @@
         <v>77</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>0</v>
@@ -62819,7 +62954,7 @@
         <v>78</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>0</v>
@@ -62833,7 +62968,7 @@
         <v>79</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>0</v>
@@ -62847,7 +62982,7 @@
         <v>80</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>0</v>
@@ -62856,7 +62991,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62864,7 +62999,7 @@
         <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>0</v>
@@ -62873,7 +63008,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62881,7 +63016,7 @@
         <v>82</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>0</v>
@@ -62890,7 +63025,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62898,7 +63033,7 @@
         <v>83</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>0</v>
@@ -62913,7 +63048,7 @@
         <v>84</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>0</v>
@@ -62928,7 +63063,7 @@
         <v>85</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>0</v>
@@ -62943,7 +63078,7 @@
         <v>86</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>0</v>
@@ -62958,7 +63093,7 @@
         <v>87</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>0</v>
@@ -62973,7 +63108,7 @@
         <v>88</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>0</v>
@@ -62988,7 +63123,7 @@
         <v>89</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>0</v>
@@ -63003,7 +63138,7 @@
         <v>90</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>0</v>
@@ -63018,7 +63153,7 @@
         <v>91</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>0</v>
@@ -63033,7 +63168,7 @@
         <v>92</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>0</v>
@@ -63048,7 +63183,7 @@
         <v>93</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>0</v>
@@ -63063,7 +63198,7 @@
         <v>94</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>0</v>
@@ -63078,7 +63213,7 @@
         <v>95</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>0</v>
@@ -63093,7 +63228,7 @@
         <v>96</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>0</v>
@@ -63108,7 +63243,7 @@
         <v>97</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>0</v>
@@ -63123,7 +63258,7 @@
         <v>98</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>0</v>
@@ -63138,7 +63273,7 @@
         <v>99</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>0</v>
@@ -63153,7 +63288,7 @@
         <v>100</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>0</v>
@@ -63168,7 +63303,7 @@
         <v>101</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>0</v>
@@ -63183,7 +63318,7 @@
         <v>102</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>0</v>
@@ -63198,7 +63333,7 @@
         <v>103</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>0</v>
@@ -63213,7 +63348,7 @@
         <v>104</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>0</v>
@@ -63228,7 +63363,7 @@
         <v>105</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>0</v>
@@ -63243,7 +63378,7 @@
         <v>106</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>0</v>
@@ -63258,7 +63393,7 @@
         <v>107</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>0</v>
@@ -63273,7 +63408,7 @@
         <v>108</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>0</v>
@@ -63288,7 +63423,7 @@
         <v>109</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>0</v>
@@ -63317,7 +63452,7 @@
   <dimension ref="A2:A43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="1" sqref="1:1 A39"/>
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -63554,7 +63689,7 @@
   <dimension ref="A2:A45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -63564,7 +63699,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -63801,7 +63936,7 @@
   <dimension ref="A2:A45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -63811,7 +63946,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64048,7 +64183,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="1" sqref="1:1 A38"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -64058,13 +64193,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64537,7 +64672,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -64547,13 +64682,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>